<commit_message>
final exam schedule mail changes
</commit_message>
<xml_diff>
--- a/FALL 19/final_exam_schedule_mail.xlsx
+++ b/FALL 19/final_exam_schedule_mail.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -42,6 +42,51 @@
     <t>anika.tabassum.cse@ulab.edu.bd</t>
   </si>
   <si>
+    <t>CSE 101</t>
+  </si>
+  <si>
+    <t>gazi.mishu.bba@ulab.edu.bd</t>
+  </si>
+  <si>
+    <t>jannatul.ferdous13.bba@ulab.edu.bd</t>
+  </si>
+  <si>
+    <t>sadia.afrin3.cse@ulab.edu.bd</t>
+  </si>
+  <si>
+    <t>tanmim.samad.cse@ulab.edu.bd</t>
+  </si>
+  <si>
+    <t>CSE 104</t>
+  </si>
+  <si>
+    <t>mansuba.tabasssum.cse@ulab.edu.bd</t>
+  </si>
+  <si>
+    <t>mutasim.billah.cse@ulab.edu.bd</t>
+  </si>
+  <si>
+    <t>CSE 208</t>
+  </si>
+  <si>
+    <t>sazeda.akter.cse@ulab.edu.bd</t>
+  </si>
+  <si>
+    <t>nafiur.rahman.cse@ulab.edu.bd</t>
+  </si>
+  <si>
+    <t>atikur.rahman.cse@ulab.edu.bd</t>
+  </si>
+  <si>
+    <t>kaniz.fatema.cse@ulab.edu.bd</t>
+  </si>
+  <si>
+    <t>Subject of Email</t>
+  </si>
+  <si>
+    <t>Final Exam Schedule</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -51,7 +96,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Mid term schedule</t>
+      <t>Final Exam Schedule</t>
     </r>
     <r>
       <rPr>
@@ -63,18 +108,9 @@
       </rPr>
       <t xml:space="preserve">
 Venue: Room 404 (Campus B)
-Date: 18.11.2019 (Monday)
-Time: 10:00 - 11:20</t>
-    </r>
-  </si>
-  <si>
-    <t>CSE 101</t>
-  </si>
-  <si>
-    <t>gazi.mishu.bba@ulab.edu.bd</t>
-  </si>
-  <si>
-    <t>jannatul.ferdous13.bba@ulab.edu.bd</t>
+Date: 8.1.2020 (Wednesday)
+Time: 10:45 - 12:45</t>
+    </r>
   </si>
   <si>
     <r>
@@ -86,7 +122,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Mid term schedule</t>
+      <t>Final Exam Schedule</t>
     </r>
     <r>
       <rPr>
@@ -98,8 +134,8 @@
       </rPr>
       <t xml:space="preserve">
 Venue: Room 301 &amp; 302 (Campus A)
-Date: 20.11.2019 (Wednesday)
-Time: 10:00 - 11:20</t>
+Date: 13.1.2020 (Monday)
+Time: 10:45 - 12:45</t>
     </r>
   </si>
   <si>
@@ -112,7 +148,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Mid term schedule</t>
+      <t>Final Exam Schedule</t>
     </r>
     <r>
       <rPr>
@@ -124,33 +160,9 @@
       </rPr>
       <t xml:space="preserve">
 Venue: Room 301 &amp; 302 (Campus A)
-Date: 20.11.2019 (Wednesday)
-Time: 8:30 - 9:50</t>
-    </r>
-  </si>
-  <si>
-    <t>sadia.afrin3.cse@ulab.edu.bd</t>
-  </si>
-  <si>
-    <t>tanmim.samad.cse@ulab.edu.bd</t>
-  </si>
-  <si>
-    <t>CSE 104</t>
-  </si>
-  <si>
-    <t>mansuba.tabasssum.cse@ulab.edu.bd</t>
-  </si>
-  <si>
-    <t>mutasim.billah.cse@ulab.edu.bd</t>
-  </si>
-  <si>
-    <t>CSE 208</t>
-  </si>
-  <si>
-    <t>sazeda.akter.cse@ulab.edu.bd</t>
-  </si>
-  <si>
-    <t>nafiur.rahman.cse@ulab.edu.bd</t>
+Date: 15.1.2020 (Wednesday)
+Time: 8:30 - 10:30</t>
+    </r>
   </si>
   <si>
     <r>
@@ -162,7 +174,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Mid term schedule</t>
+      <t>Final Exam Schedule</t>
     </r>
     <r>
       <rPr>
@@ -174,8 +186,8 @@
       </rPr>
       <t xml:space="preserve">
 Venue: Room PB - 105 (Permanent Campus)
-Date: 19.11.2019 (Tuesday)
-Time: 4:10 - 5:30</t>
+Date: 12.1.2020 (Sunday)
+Time: 1:15 -3:15</t>
     </r>
   </si>
   <si>
@@ -188,7 +200,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Mid term schedule</t>
+      <t>Final Exam Schedule</t>
     </r>
     <r>
       <rPr>
@@ -200,15 +212,9 @@
       </rPr>
       <t xml:space="preserve">
 Venue: Room PB - 105 (Permanent Campus)
-Date: 17.11.2019 (Sunday)
-Time: 11:30 - 12:50</t>
-    </r>
-  </si>
-  <si>
-    <t>atikur.rahman.cse@ulab.edu.bd</t>
-  </si>
-  <si>
-    <t>kaniz.fatema.cse@ulab.edu.bd</t>
+Date: 14.1.2020 (Tuesday)
+Time: 3:30 - 5:30</t>
+    </r>
   </si>
   <si>
     <r>
@@ -220,7 +226,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Mid term schedule</t>
+      <t>Final Exam Schedule</t>
     </r>
     <r>
       <rPr>
@@ -232,22 +238,16 @@
       </rPr>
       <t xml:space="preserve">
 Venue: Room PB - 106 (Permanent Campus)
-Date: 19.11.2019 (Tuesday)
-Time: 2:40 - 4:00</t>
-    </r>
-  </si>
-  <si>
-    <t>Subject of Email</t>
-  </si>
-  <si>
-    <t>Mid term schedule</t>
+Date: 14.1.2020 (Tuesday)
+Time: 1:15 -3:15</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,7 +272,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -280,14 +280,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -295,6 +325,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -341,7 +379,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -373,9 +411,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -407,6 +446,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -582,14 +622,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="3" max="3" width="47" customWidth="1"/>
@@ -598,27 +638,27 @@
     <col min="6" max="6" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>27</v>
+      <c r="F1" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60">
+    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -632,110 +672,110 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="60">
-      <c r="A3" t="s">
-        <v>9</v>
       </c>
       <c r="B3">
         <v>8</v>
       </c>
       <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="60">
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="60">
-      <c r="A5" t="s">
-        <v>16</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="60">
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
         <v>22</v>
       </c>
-      <c r="F6" t="s">
-        <v>28</v>
-      </c>
     </row>
-    <row r="7" spans="1:6" ht="60">
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -745,24 +785,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated final exam schedule mail
</commit_message>
<xml_diff>
--- a/FALL 19/final_exam_schedule_mail.xlsx
+++ b/FALL 19/final_exam_schedule_mail.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -211,43 +211,43 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Venue: Room PB - 105 (Permanent Campus)
-Date: 14.1.2020 (Tuesday)
-Time: 3:30 - 5:30</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Final Exam Schedule</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
 Venue: Room PB - 106 (Permanent Campus)
 Date: 14.1.2020 (Tuesday)
 Time: 1:15 -3:15</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Final Exam Schedule</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Venue: Room PB - 105 (Permanent Campus)
+Date: 6.1.2020 (Monday)
+Time: 10:45 - 12:45</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,7 +379,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -411,10 +411,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -446,7 +445,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -622,14 +620,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="3" max="3" width="47" customWidth="1"/>
@@ -638,7 +636,7 @@
     <col min="6" max="6" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -658,7 +656,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="60">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -678,7 +676,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="60">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -698,7 +696,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="60">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -718,7 +716,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="60">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -738,7 +736,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="60">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -752,13 +750,13 @@
         <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="60">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -772,7 +770,7 @@
         <v>20</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" t="s">
         <v>22</v>
@@ -785,24 +783,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>